<commit_message>
go home, gio ong ngoai
</commit_message>
<xml_diff>
--- a/BWTracker.xlsx
+++ b/BWTracker.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
   <si>
     <t>day</t>
   </si>
@@ -132,6 +132,36 @@
   </si>
   <si>
     <t>03:28:43</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>import data to database</t>
+  </si>
+  <si>
+    <t>import data from 2 excel file ENGRVW &amp; AR to odc database</t>
+  </si>
+  <si>
+    <t>02:28:10</t>
+  </si>
+  <si>
+    <t>00:30:10</t>
+  </si>
+  <si>
+    <t>00:15:42</t>
+  </si>
+  <si>
+    <t>01:23:38</t>
+  </si>
+  <si>
+    <t>00:44:08</t>
+  </si>
+  <si>
+    <t>00:53:04</t>
+  </si>
+  <si>
+    <t>01:19:52</t>
   </si>
 </sst>
 </file>
@@ -586,7 +616,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:EL5"/>
+  <dimension ref="A1:EL12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
@@ -1247,6 +1277,377 @@
         <v>18</v>
       </c>
       <c r="Q5" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:142" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E6" s="2">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7</v>
+      </c>
+      <c r="G6" s="2">
+        <v>23</v>
+      </c>
+      <c r="H6" s="2">
+        <v>51</v>
+      </c>
+      <c r="I6" s="2">
+        <v>9</v>
+      </c>
+      <c r="J6" s="2">
+        <v>52</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:142" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E7" s="2">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2">
+        <v>59</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2">
+        <v>29</v>
+      </c>
+      <c r="K7" s="2">
+        <v>11</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:142" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="2">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E8" s="2">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <v>40</v>
+      </c>
+      <c r="H8" s="2">
+        <v>49</v>
+      </c>
+      <c r="I8" s="2">
+        <v>10</v>
+      </c>
+      <c r="J8" s="2">
+        <v>56</v>
+      </c>
+      <c r="K8" s="2">
+        <v>32</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:142" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E9" s="2">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2">
+        <v>12</v>
+      </c>
+      <c r="H9" s="2">
+        <v>53</v>
+      </c>
+      <c r="I9" s="2">
+        <v>12</v>
+      </c>
+      <c r="J9" s="2">
+        <v>36</v>
+      </c>
+      <c r="K9" s="2">
+        <v>31</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:142" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="2">
+        <v>11</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E10" s="2">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2">
+        <v>48</v>
+      </c>
+      <c r="I10" s="2">
+        <v>13</v>
+      </c>
+      <c r="J10" s="2">
+        <v>58</v>
+      </c>
+      <c r="K10" s="2">
+        <v>57</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:142" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E11" s="2">
+        <v>28</v>
+      </c>
+      <c r="F11" s="2">
+        <v>14</v>
+      </c>
+      <c r="G11" s="2">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2">
+        <v>27</v>
+      </c>
+      <c r="I11" s="2">
+        <v>15</v>
+      </c>
+      <c r="J11" s="2">
+        <v>7</v>
+      </c>
+      <c r="K11" s="2">
+        <v>32</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:142" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2017</v>
+      </c>
+      <c r="E12" s="2">
+        <v>28</v>
+      </c>
+      <c r="F12" s="2">
+        <v>15</v>
+      </c>
+      <c r="G12" s="2">
+        <v>17</v>
+      </c>
+      <c r="H12" s="2">
+        <v>45</v>
+      </c>
+      <c r="I12" s="2">
+        <v>16</v>
+      </c>
+      <c r="J12" s="2">
+        <v>37</v>
+      </c>
+      <c r="K12" s="2">
+        <v>38</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>